<commit_message>
Battery mount and full weight calculation
</commit_message>
<xml_diff>
--- a/Frame/Weight calculation.xlsx
+++ b/Frame/Weight calculation.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKAR\Dron\SOLIDWORKS\Rama\Wersja 3 - druk FDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKAR\Dron\Github\drone\Frame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6316AA-3B22-4A5E-B41E-1F4393B67304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F46F47-5F9A-4BEC-AF4C-72EF28905BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Frame" sheetId="1" r:id="rId1"/>
+    <sheet name="Drone" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>L.p.</t>
   </si>
@@ -62,12 +63,6 @@
     <t>Fixed tripod connector 10mm</t>
   </si>
   <si>
-    <t>Motor_mount_14mm</t>
-  </si>
-  <si>
-    <t>Frame pipe 14x250x2</t>
-  </si>
-  <si>
     <t>Pipe clamp 14mm</t>
   </si>
   <si>
@@ -81,6 +76,39 @@
   </si>
   <si>
     <t>Frame pipe 10x120x1</t>
+  </si>
+  <si>
+    <t>Frame pipe 14x175x2</t>
+  </si>
+  <si>
+    <t>Battety mount left</t>
+  </si>
+  <si>
+    <t>Battety mount right</t>
+  </si>
+  <si>
+    <t>Battety mount front</t>
+  </si>
+  <si>
+    <t>Motor mount 14mm</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Cube Orange</t>
+  </si>
+  <si>
+    <t>Halybro Telemetry 433MHz</t>
+  </si>
+  <si>
+    <t>Wi-Fi antena</t>
+  </si>
+  <si>
+    <t>ESC Afro 40A</t>
   </si>
 </sst>
 </file>
@@ -370,6 +398,57 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-9FAE-4701-8581-8F96C8D58B0B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -428,37 +507,46 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$3:$C$12</c:f>
+              <c:f>Frame!$C$3:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Battety mount front</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Battety mount right</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Battety mount left</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Frame pipe 10x120x1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Fixed tripod connector 10mm</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Frame pipe 10x300x1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Pipe clamp 14mm top</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Landing gear 10mm</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Motor_mount_14mm</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>Motor mount 14mm</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Frame plane top 1mm</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Frame plane bot 1mm</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Frame pipe 14x250x2</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>Frame pipe 14x175x2</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Pipe clamp 14mm</c:v>
                 </c:pt>
               </c:strCache>
@@ -466,39 +554,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$F$3:$F$12</c:f>
+              <c:f>Frame!$F$3:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>21.72</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>26.48</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>27.14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>31.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>34.36</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>50.16</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>58.67</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>63.09</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>120.64</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>136.63999999999999</c:v>
+                <c:pt idx="11">
+                  <c:v>84.44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>168.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,37 +767,46 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$3:$C$12</c:f>
+              <c:f>Frame!$C$3:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Battety mount front</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Battety mount right</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Battety mount left</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Frame pipe 10x120x1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Fixed tripod connector 10mm</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Frame pipe 10x300x1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Pipe clamp 14mm top</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Landing gear 10mm</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Motor_mount_14mm</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>Motor mount 14mm</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Frame plane top 1mm</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Frame plane bot 1mm</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Frame pipe 14x250x2</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>Frame pipe 14x175x2</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Pipe clamp 14mm</c:v>
                 </c:pt>
               </c:strCache>
@@ -708,39 +814,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$F$3:$F$12</c:f>
+              <c:f>Frame!$F$3:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>21.72</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>26.48</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>27.14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>31.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>34.36</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>50.16</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>58.67</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>63.09</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>120.64</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>136.63999999999999</c:v>
+                <c:pt idx="11">
+                  <c:v>84.44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>168.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1998,15 +2113,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2034,15 +2149,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2333,10 +2448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,17 +2483,17 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5.43</v>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.92</v>
       </c>
       <c r="F3">
         <f>D3*E3</f>
-        <v>21.72</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -2386,17 +2501,17 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>6.62</v>
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14.05</v>
       </c>
       <c r="F4">
         <f>D4*E4</f>
-        <v>26.48</v>
+        <v>14.05</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -2404,17 +2519,17 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>13.57</v>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>14.05</v>
       </c>
       <c r="F5">
         <f>D5*E5</f>
-        <v>27.14</v>
+        <v>14.05</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -2422,17 +2537,17 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3.95</v>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5.43</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>31.6</v>
+        <v>21.72</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2440,17 +2555,17 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>8.59</v>
+        <v>6.62</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>34.36</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -2458,17 +2573,17 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>12.54</v>
+        <v>13.57</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>50.16</v>
+        <v>27.14</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -2476,17 +2591,17 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>58.67</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.95</v>
       </c>
       <c r="F9">
         <f>D9*E9</f>
-        <v>58.67</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -2494,17 +2609,17 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>63.09</v>
+        <v>8.59</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>63.09</v>
+        <v>34.36</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -2512,17 +2627,17 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11">
-        <v>30.16</v>
+        <v>12.54</v>
       </c>
       <c r="F11">
         <f>D11*E11</f>
-        <v>120.64</v>
+        <v>50.16</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -2530,30 +2645,470 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1">
-        <v>17.079999999999998</v>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>58.67</v>
       </c>
       <c r="F12">
         <f>D12*E12</f>
-        <v>136.63999999999999</v>
+        <v>58.67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>63.09</v>
+      </c>
+      <c r="F13">
+        <f>D13*E13</f>
+        <v>63.09</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>21.11</v>
+      </c>
+      <c r="F14">
+        <f>D14*E14</f>
+        <v>84.44</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <v>21.02</v>
+      </c>
       <c r="F15">
-        <f>SUM(F3:F14)</f>
-        <v>570.5</v>
+        <f>D15*E15</f>
+        <v>168.16</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f>SUM(F3:F15)</f>
+        <v>596.84</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F12">
-    <sortCondition ref="F12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F15">
+    <sortCondition ref="F15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F36D7B6-4377-43C1-9083-4C0940A25C9D}">
+  <dimension ref="B2:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.92</v>
+      </c>
+      <c r="F3">
+        <f>D3*E3</f>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14.05</v>
+      </c>
+      <c r="F4">
+        <f>D4*E4</f>
+        <v>14.05</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>14.05</v>
+      </c>
+      <c r="F5">
+        <f>D5*E5</f>
+        <v>14.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5.43</v>
+      </c>
+      <c r="F6">
+        <f>D6*E6</f>
+        <v>21.72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>6.62</v>
+      </c>
+      <c r="F7">
+        <f>D7*E7</f>
+        <v>26.48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>13.57</v>
+      </c>
+      <c r="F8">
+        <f>D8*E8</f>
+        <v>27.14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="F9">
+        <f>D9*E9</f>
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>8.59</v>
+      </c>
+      <c r="F10">
+        <f>D10*E10</f>
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>12.54</v>
+      </c>
+      <c r="F11">
+        <f>D11*E11</f>
+        <v>50.16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>58.67</v>
+      </c>
+      <c r="F12">
+        <f>D12*E12</f>
+        <v>58.67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>63.09</v>
+      </c>
+      <c r="F13">
+        <f>D13*E13</f>
+        <v>63.09</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>21.11</v>
+      </c>
+      <c r="F14">
+        <f>D14*E14</f>
+        <v>84.44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <v>21.02</v>
+      </c>
+      <c r="F15">
+        <f>D15*E15</f>
+        <v>168.16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>907</v>
+      </c>
+      <c r="F16">
+        <f>D16*E16</f>
+        <v>907</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>67</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F21" si="0">D17*E17</f>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>73</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>26.5</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f>SUM(F3:F21)</f>
+        <v>1989.8400000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Export of show model and some minor frame changes
</commit_message>
<xml_diff>
--- a/Frame/Weight calculation.xlsx
+++ b/Frame/Weight calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKAR\Dron\Github\drone\Frame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F46F47-5F9A-4BEC-AF4C-72EF28905BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFA383F-F344-4A5A-BA5D-37228A700D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frame" sheetId="1" r:id="rId1"/>
@@ -115,12 +115,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -144,9 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -179,6 +189,38 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Wykres</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> rozkładu masy ramy</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -216,6 +258,7 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="2"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -418,6 +461,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-7CD6-4B7C-A132-379BE7267502}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -433,6 +481,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-7CD6-4B7C-A132-379BE7267502}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -449,8 +502,76 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-7CD6-4B7C-A132-379BE7267502}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8042397075938319E-3"/>
+                  <c:y val="-7.3142830814729068E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-81B6-4451-B0B5-7A6AB7EB7E15}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8042397075938319E-3"/>
+                  <c:y val="-3.9619033357978242E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-81B6-4451-B0B5-7A6AB7EB7E15}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8042397075938319E-3"/>
+                  <c:y val="-3.0476179506137166E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-81B6-4451-B0B5-7A6AB7EB7E15}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -481,26 +602,12 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
@@ -608,15 +715,15 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
+          <c:showLeaderLines val="0"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
+        <c:holeSize val="30"/>
       </c:doughnutChart>
       <c:spPr>
         <a:noFill/>
@@ -716,6 +823,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Wykres</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> rozkładu masy ramy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1031,6 +1169,466 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wykres rozkładu masy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> drona</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Drone!$C$3:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Battety mount front</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Battety mount right</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Battety mount left</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Halybro Telemetry 433MHz</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Wi-Fi antena</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Frame pipe 10x120x1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fixed tripod connector 10mm</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Frame pipe 10x300x1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Pipe clamp 14mm top</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Landing gear 10mm</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Motor mount 14mm</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Frame plane top 1mm</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Frame plane bot 1mm</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Cube Orange</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Frame pipe 14x175x2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ESC Afro 40A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Pipe clamp 14mm</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Motor</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Battery</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Drone!$F$3:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.67</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63.09</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84.44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>168.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>907</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A4D2-439C-86F0-F20E97AC44F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1432158144"/>
+        <c:axId val="1628469344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1432158144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1628469344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1628469344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1432158144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1111,6 +1709,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -1606,6 +2244,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2118,10 +3259,10 @@
       <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2177,6 +3318,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4501CBE7-8A11-AA15-277A-3733CAACB08F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2451,7 +3633,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2492,7 +3674,7 @@
         <v>2.92</v>
       </c>
       <c r="F3">
-        <f>D3*E3</f>
+        <f t="shared" ref="F3:F15" si="0">D3*E3</f>
         <v>2.92</v>
       </c>
     </row>
@@ -2510,7 +3692,7 @@
         <v>14.05</v>
       </c>
       <c r="F4">
-        <f>D4*E4</f>
+        <f t="shared" si="0"/>
         <v>14.05</v>
       </c>
     </row>
@@ -2528,7 +3710,7 @@
         <v>14.05</v>
       </c>
       <c r="F5">
-        <f>D5*E5</f>
+        <f t="shared" si="0"/>
         <v>14.05</v>
       </c>
     </row>
@@ -2546,7 +3728,7 @@
         <v>5.43</v>
       </c>
       <c r="F6">
-        <f>D6*E6</f>
+        <f t="shared" si="0"/>
         <v>21.72</v>
       </c>
     </row>
@@ -2564,7 +3746,7 @@
         <v>6.62</v>
       </c>
       <c r="F7">
-        <f>D7*E7</f>
+        <f t="shared" si="0"/>
         <v>26.48</v>
       </c>
     </row>
@@ -2582,7 +3764,7 @@
         <v>13.57</v>
       </c>
       <c r="F8">
-        <f>D8*E8</f>
+        <f t="shared" si="0"/>
         <v>27.14</v>
       </c>
     </row>
@@ -2600,7 +3782,7 @@
         <v>3.95</v>
       </c>
       <c r="F9">
-        <f>D9*E9</f>
+        <f t="shared" si="0"/>
         <v>31.6</v>
       </c>
     </row>
@@ -2618,7 +3800,7 @@
         <v>8.59</v>
       </c>
       <c r="F10">
-        <f>D10*E10</f>
+        <f t="shared" si="0"/>
         <v>34.36</v>
       </c>
     </row>
@@ -2636,7 +3818,7 @@
         <v>12.54</v>
       </c>
       <c r="F11">
-        <f>D11*E11</f>
+        <f t="shared" si="0"/>
         <v>50.16</v>
       </c>
     </row>
@@ -2654,7 +3836,7 @@
         <v>58.67</v>
       </c>
       <c r="F12">
-        <f>D12*E12</f>
+        <f t="shared" si="0"/>
         <v>58.67</v>
       </c>
     </row>
@@ -2672,7 +3854,7 @@
         <v>63.09</v>
       </c>
       <c r="F13">
-        <f>D13*E13</f>
+        <f t="shared" si="0"/>
         <v>63.09</v>
       </c>
     </row>
@@ -2690,7 +3872,7 @@
         <v>21.11</v>
       </c>
       <c r="F14">
-        <f>D14*E14</f>
+        <f t="shared" si="0"/>
         <v>84.44</v>
       </c>
     </row>
@@ -2708,12 +3890,12 @@
         <v>21.02</v>
       </c>
       <c r="F15">
-        <f>D15*E15</f>
+        <f t="shared" si="0"/>
         <v>168.16</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17">
+      <c r="F17" s="2">
         <f>SUM(F3:F15)</f>
         <v>596.84</v>
       </c>
@@ -2723,7 +3905,8 @@
     <sortCondition ref="F15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2732,7 +3915,7 @@
   <dimension ref="B2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,17 +4001,17 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>5.43</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>21.72</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2836,17 +4019,17 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>6.62</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>26.48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -2854,17 +4037,17 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>13.57</v>
+        <v>5.43</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>27.14</v>
+        <v>21.72</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -2872,17 +4055,17 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3.95</v>
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>6.62</v>
       </c>
       <c r="F9">
         <f>D9*E9</f>
-        <v>31.6</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -2890,17 +4073,17 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>8.59</v>
+        <v>13.57</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>34.36</v>
+        <v>27.14</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -2908,17 +4091,17 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>12.54</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3.95</v>
       </c>
       <c r="F11">
         <f>D11*E11</f>
-        <v>50.16</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -2926,17 +4109,17 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>58.67</v>
+        <v>8.59</v>
       </c>
       <c r="F12">
         <f>D12*E12</f>
-        <v>58.67</v>
+        <v>34.36</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -2944,17 +4127,17 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>63.09</v>
+        <v>12.54</v>
       </c>
       <c r="F13">
         <f>D13*E13</f>
-        <v>63.09</v>
+        <v>50.16</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -2962,17 +4145,17 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>21.11</v>
+        <v>58.67</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>84.44</v>
+        <v>58.67</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -2980,17 +4163,17 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1">
-        <v>21.02</v>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>63.09</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>168.16</v>
+        <v>63.09</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -2998,17 +4181,17 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>907</v>
+        <v>73</v>
       </c>
       <c r="F16">
         <f>D16*E16</f>
-        <v>907</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -3016,17 +4199,17 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17">
-        <v>67</v>
+        <v>21.11</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F21" si="0">D17*E17</f>
-        <v>268</v>
+        <f>D17*E17</f>
+        <v>84.44</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -3034,17 +4217,17 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>73</v>
+        <v>26.5</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>73</v>
+        <f>D18*E18</f>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -3052,17 +4235,17 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="E19" s="1">
+        <v>21.02</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f>D19*E19</f>
+        <v>168.16</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -3070,17 +4253,17 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>D20*E20</f>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -3088,27 +4271,31 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>26.5</v>
+        <v>907</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>106</v>
+        <f>D21*E21</f>
+        <v>907</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F23">
+      <c r="F23" s="2">
         <f>SUM(F3:F21)</f>
         <v>1989.8400000000001</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F21">
+    <sortCondition ref="F3:F21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>